<commit_message>
🔧 Add time series forecasting with SARIMA and Prophet + visualize predictions
</commit_message>
<xml_diff>
--- a/data/상품별공급량_MJ.xlsx
+++ b/data/상품별공급량_MJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_Project\상품별월공급량예측모델\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8B5E5E-4110-437D-B37C-6413D2C6CC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{799C7C54-756E-48D5-9CCE-C8B3094A73FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -202,7 +202,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -237,9 +237,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1334,7 +1331,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표1" displayName="표1" ref="A1:X150" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="표1" displayName="표1" ref="A1:X148" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="날짜" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="연" dataDxfId="22"/>
@@ -1634,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI150"/>
+  <dimension ref="A1:AI148"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F155" sqref="F155"/>
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -12965,92 +12962,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A149" s="2">
-        <v>45748</v>
-      </c>
-      <c r="B149" s="11">
-        <v>2025</v>
-      </c>
-      <c r="C149" s="11">
-        <v>4</v>
-      </c>
-      <c r="D149" s="11">
-        <v>14.9</v>
-      </c>
-      <c r="E149" s="11"/>
-      <c r="F149" s="11"/>
-      <c r="G149" s="11"/>
-      <c r="H149" s="8"/>
-      <c r="I149" s="11">
-        <f t="shared" ref="I149:I150" si="6">SUM(U149:U149)</f>
-        <v>0</v>
-      </c>
-      <c r="J149" s="11"/>
-      <c r="K149" s="11"/>
-      <c r="L149" s="8"/>
-      <c r="M149" s="8"/>
-      <c r="N149" s="8"/>
-      <c r="O149" s="8"/>
-      <c r="P149" s="11"/>
-      <c r="Q149" s="11"/>
-      <c r="R149" s="11"/>
-      <c r="S149" s="8"/>
-      <c r="T149" s="8"/>
-      <c r="U149" s="8"/>
-      <c r="V149" s="11"/>
-      <c r="W149" s="11">
-        <f>SUM(표1[[#This Row],[취사용]:[주한미군]])</f>
-        <v>0</v>
-      </c>
-      <c r="X149" s="12">
-        <f t="shared" ref="X149:X150" si="7">V149-W149</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A150" s="10">
-        <v>45778</v>
-      </c>
-      <c r="B150" s="11">
-        <v>2025</v>
-      </c>
-      <c r="C150" s="11">
-        <v>5</v>
-      </c>
-      <c r="D150" s="11">
-        <v>18.100000000000001</v>
-      </c>
-      <c r="E150" s="11"/>
-      <c r="F150" s="11"/>
-      <c r="G150" s="11"/>
-      <c r="H150" s="8"/>
-      <c r="I150" s="11">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J150" s="11"/>
-      <c r="K150" s="11"/>
-      <c r="L150" s="8"/>
-      <c r="M150" s="8"/>
-      <c r="N150" s="8"/>
-      <c r="O150" s="8"/>
-      <c r="P150" s="11"/>
-      <c r="Q150" s="11"/>
-      <c r="R150" s="11"/>
-      <c r="S150" s="8"/>
-      <c r="T150" s="8"/>
-      <c r="U150" s="8"/>
-      <c r="V150" s="11"/>
-      <c r="W150" s="11">
-        <f>SUM(표1[[#This Row],[취사용]:[주한미군]])</f>
-        <v>0</v>
-      </c>
-      <c r="X150" s="12">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>